<commit_message>
add cache of rows to improve random access/rewind perfs
</commit_message>
<xml_diff>
--- a/t/regression/xlsx_files/data01.xlsx
+++ b/t/regression/xlsx_files/data01.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="20412"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="100" windowWidth="16100" windowHeight="7360"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="16095" windowHeight="7365"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12,7 +12,7 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
     <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
   <si>
     <t>Foo</t>
   </si>
@@ -73,6 +73,15 @@
   </si>
   <si>
     <t>This is a unicode string €</t>
+  </si>
+  <si>
+    <t>+++Hihi!</t>
+  </si>
+  <si>
+    <t>(+c7+)</t>
+  </si>
+  <si>
+    <t>bar</t>
   </si>
 </sst>
 </file>
@@ -123,15 +132,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -420,41 +435,46 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="1" customFormat="1"/>
-    <row r="3" spans="1:3">
+    <row r="2" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
-        <v>4</v>
+        <v>42</v>
       </c>
       <c r="C3">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <f>5+5</f>
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:3">
+      <c r="D5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
     </row>
   </sheetData>
@@ -469,47 +489,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1">
-      <c r="A4">
-        <v>123</v>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -522,20 +517,58 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>123</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
* use sheet-index is now the index of sheet declaration * ignore missing files by default
</commit_message>
<xml_diff>
--- a/t/regression/xlsx_files/data01.xlsx
+++ b/t/regression/xlsx_files/data01.xlsx
@@ -7,10 +7,10 @@
     <workbookView xWindow="240" yWindow="105" windowWidth="16095" windowHeight="7365"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="feuillea"/>
+    <sheet name="Sheet2" sheetId="2" r:id="feuilleb"/>
+    <sheet name="Sheet3" sheetId="3" r:id="feuillec"/>
+    <sheet name="Sheet4" sheetId="4" r:id="feuilled"/>
   </sheets>
   <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>

</xml_diff>